<commit_message>
debtor result - column heights issues
</commit_message>
<xml_diff>
--- a/common/data/DebtorsReportTemplate.xlsx
+++ b/common/data/DebtorsReportTemplate.xlsx
@@ -292,7 +292,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0" hidden="1"/>
@@ -337,6 +337,9 @@
       <protection locked="0" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0" hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -671,7 +674,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -713,7 +716,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -736,10 +739,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -762,20 +765,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="9.1999999999999993" customHeight="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:15" ht="14.45" customHeight="1">
       <c r="I2"/>
@@ -817,7 +820,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="90.6" customHeight="1">
+    <row r="7" spans="1:15" ht="74.25" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -862,22 +865,22 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="12.75" hidden="1" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="21"/>
-    </row>
-    <row r="9" spans="1:15" ht="12.75" hidden="1" customHeight="1">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="22"/>
+    </row>
+    <row r="9" spans="1:15" ht="24" hidden="1" customHeight="1">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -919,57 +922,57 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="29.1" customHeight="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17" t="s">
+    <row r="10" spans="1:15" s="18" customFormat="1" ht="0.75" customHeight="1">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+      <c r="O10"/>
+    </row>
+    <row r="11" spans="1:15" ht="29.1" customHeight="1">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16" t="e">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="K10" s="17" t="e">
+      <c r="K11" s="17" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="L10" s="17" t="e">
+      <c r="L11" s="17" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="M10" s="17" t="e">
+      <c r="M11" s="17" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="N10" s="17" t="e">
+      <c r="N11" s="17" t="e">
         <f>SUM(#REF!)</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="17.25" customHeight="1">
-      <c r="A12" s="10" t="s">
+    <row r="13" spans="1:15" ht="17.25" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:15" ht="12.4" customHeight="1">
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
@@ -980,38 +983,34 @@
       <c r="I13" s="10"/>
       <c r="J13" s="10"/>
       <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="O13"/>
-    </row>
-    <row r="14" spans="1:15" ht="18.75">
-      <c r="B14" s="11" t="s">
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:15" ht="12.4" customHeight="1">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="O14"/>
+    </row>
+    <row r="15" spans="1:15" ht="18.75">
+      <c r="B15" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="O14"/>
-    </row>
-    <row r="15" spans="1:15" ht="18.75">
-      <c r="B15" s="12" t="s">
-        <v>26</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12" t="s">
-        <v>26</v>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
@@ -1020,13 +1019,17 @@
       <c r="O15"/>
     </row>
     <row r="16" spans="1:15" ht="18.75">
-      <c r="B16" s="12"/>
+      <c r="B16" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="H16" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -1048,17 +1051,13 @@
       <c r="O17"/>
     </row>
     <row r="18" spans="2:15" ht="18.75">
-      <c r="B18" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="12"/>
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="H18" s="12"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -1067,7 +1066,7 @@
     </row>
     <row r="19" spans="2:15" ht="18.75">
       <c r="B19" s="12" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C19" s="12"/>
       <c r="D19" s="12"/>
@@ -1075,7 +1074,7 @@
       <c r="F19" s="12"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
@@ -1084,33 +1083,35 @@
       <c r="O19"/>
     </row>
     <row r="20" spans="2:15" ht="18.75">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20"/>
-      <c r="N20"/>
+      <c r="B20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="13"/>
       <c r="O20"/>
     </row>
-    <row r="21" spans="2:15">
-      <c r="B21"/>
-      <c r="C21"/>
-      <c r="D21"/>
-      <c r="E21"/>
-      <c r="F21"/>
-      <c r="G21"/>
-      <c r="H21"/>
-      <c r="I21"/>
-      <c r="J21"/>
-      <c r="K21"/>
-      <c r="L21"/>
+    <row r="21" spans="2:15" ht="18.75">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
@@ -1131,6 +1132,22 @@
       <c r="N22"/>
       <c r="O22"/>
     </row>
+    <row r="23" spans="2:15">
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Revert "debtor result - column heights issues"
This reverts commit bae8c49167701cb4b7d818f21bc66de509bca50c.

# Conflicts:
#	common/data/DebtorsReportTemplate.xlsx
#	frontend/modules/office/controllers/DebtorController.php
</commit_message>
<xml_diff>
--- a/common/data/DebtorsReportTemplate.xlsx
+++ b/common/data/DebtorsReportTemplate.xlsx
@@ -140,7 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -214,6 +214,13 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="8"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -354,8 +361,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -677,7 +684,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -719,7 +726,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -745,7 +752,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -823,7 +830,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="74.25" customHeight="1">
+    <row r="7" spans="1:15" ht="96.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -925,21 +932,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="18" customFormat="1" ht="18.75" hidden="1">
+    <row r="10" spans="1:15" s="18" customFormat="1" ht="1.5" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10"/>
     </row>
     <row r="11" spans="1:15" ht="29.1" customHeight="1">
       <c r="A11" s="14"/>
@@ -953,26 +961,11 @@
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
-      <c r="J11" s="16" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K11" s="17" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="L11" s="17" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="M11" s="17" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N11" s="17" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1">
       <c r="A13" s="10" t="s">

</xml_diff>

<commit_message>
borders for debtor report table
</commit_message>
<xml_diff>
--- a/common/data/DebtorsReportTemplate.xlsx
+++ b/common/data/DebtorsReportTemplate.xlsx
@@ -186,7 +186,8 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <sz val="14"/>
@@ -299,7 +300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0" hidden="1"/>
@@ -361,9 +362,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0" hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0" hidden="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0" hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -684,7 +687,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -726,7 +729,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -752,7 +755,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -934,17 +937,17 @@
     </row>
     <row r="10" spans="1:15" s="18" customFormat="1" ht="1.5" customHeight="1">
       <c r="A10" s="23"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="25"/>
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
       <c r="O10"/>

</xml_diff>